<commit_message>
refazendo a função de gerar gabarito
</commit_message>
<xml_diff>
--- a/slither/0.8.0_smartbugs-curated/0.8.0_slither_smartbugs-curated_dasp_soma.xlsx
+++ b/slither/0.8.0_smartbugs-curated/0.8.0_slither_smartbugs-curated_dasp_soma.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,67 +447,67 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>index</t>
+          <t>Ignore</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2346</v>
+        <v>690</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Ignore</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>690</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>time_manipulation</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>46</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>time_manipulation</t>
+          <t>access_control</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>access_control</t>
+          <t>reentrancy</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7">
@@ -516,46 +516,46 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>reentrancy</t>
+          <t>unchecked_low_calls</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>unchecked_low_calls</t>
+          <t>denial_service</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>denial_service</t>
+          <t>arithmetic</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>arithmetic</t>
+          <t>bad_randomness</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -568,7 +568,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>bad_randomness</t>
+          <t>front_running</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -577,27 +577,14 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>front_running</t>
+          <t>short_addresses</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>short_addresses</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>